<commit_message>
Setup css style sheet structures, start building new page layout in HTML - incorporating Boiler plate HTML and integrating XILIR layouts. Clean up HTML markup.
</commit_message>
<xml_diff>
--- a/timesheet/anthonyalbertyn-timesheet.xlsx
+++ b/timesheet/anthonyalbertyn-timesheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DATE</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Review of the theme, screenshots, html5 boilerplate review, setup of folders and content in GIT</t>
+  </si>
+  <si>
+    <t>Setup css style sheet structures, start building new page layout in HTML - incorporating Boiler plate HTML and integrating XILIR layouts. Clean up HTML markup.</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -461,6 +464,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="6">
+        <v>41948</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Clean up HTML, introduce some CSS and partially integrate 960 grid system
</commit_message>
<xml_diff>
--- a/timesheet/anthonyalbertyn-timesheet.xlsx
+++ b/timesheet/anthonyalbertyn-timesheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25300" yWindow="2580" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="-27700" yWindow="2080" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DATE</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Setup css style sheet structures, start building new page layout in HTML - incorporating Boiler plate HTML and integrating XILIR layouts. Clean up HTML markup.</t>
+  </si>
+  <si>
+    <t>Clean up HTML and partially integrate 960 grid system</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -475,6 +478,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6">
+        <v>41949</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>